<commit_message>
Tested PCB for force sensor, updated excel test sheet and the Arduino script
</commit_message>
<xml_diff>
--- a/Software/Force Sensor Testing.xlsx
+++ b/Software/Force Sensor Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiara\Desktop\Projects\Gripper Arm - ROBOTICS CLUB\Gripper-Arm\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD74DB2F-1651-47D3-AB0F-EEB486FE2857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B3DFDB-312F-4E97-B52A-D2819129A794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Force (N)</t>
+    <t>Load (kg)</t>
   </si>
   <si>
-    <t>Voltage (V)</t>
+    <t>Voltage tst 1 (V)</t>
   </si>
   <si>
-    <t>ADC</t>
+    <t>FSR_2 Input test</t>
   </si>
 </sst>
 </file>
@@ -385,26 +385,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4DA9E8-322B-499C-8602-612DAACEC321}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="3" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.76953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>0.2</v>
+      </c>
+      <c r="B5">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>0.3</v>
+      </c>
+      <c r="B6">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>0.6</v>
+      </c>
+      <c r="B9">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>0.7</v>
+      </c>
+      <c r="B10">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>0.8</v>
+      </c>
+      <c r="B11">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>0.9</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>1.5</v>
+      </c>
+      <c r="B14">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A15">
         <v>2</v>
+      </c>
+      <c r="B15">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>2.5</v>
+      </c>
+      <c r="B16">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>3.5</v>
+      </c>
+      <c r="B18">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>7.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>4.5</v>
+      </c>
+      <c r="B20">
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on current sensing
</commit_message>
<xml_diff>
--- a/Software/Force Sensor Testing.xlsx
+++ b/Software/Force Sensor Testing.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiara\Desktop\Projects\Gripper Arm - ROBOTICS CLUB\Gripper-Arm\Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gripper-Arm\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B3DFDB-312F-4E97-B52A-D2819129A794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4D81A-8C1B-463E-B5A4-A6319BBE1BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Load (kg)</t>
   </si>
@@ -34,6 +46,18 @@
   </si>
   <si>
     <t>FSR_2 Input test</t>
+  </si>
+  <si>
+    <t>Current Sensor Testing</t>
+  </si>
+  <si>
+    <t>Current (A)</t>
+  </si>
+  <si>
+    <t>ADC Reading</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
   </si>
 </sst>
 </file>
@@ -86,6 +110,1011 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.1014873140857392E-3"/>
+                  <c:y val="-0.14856262758821814"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$11:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$11:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9EBA-498E-B789-B87FD5429580}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="544097440"/>
+        <c:axId val="544091680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="544097440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544091680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="544091680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544097440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>73818</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>111918</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{568E73C6-D458-9DB6-1EF1-75C199EE0BF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,21 +1416,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4DA9E8-322B-499C-8602-612DAACEC321}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="3" width="13.76953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -409,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0</v>
       </c>
@@ -417,7 +1446,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -425,7 +1454,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -433,7 +1462,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -441,7 +1470,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.4</v>
       </c>
@@ -449,7 +1478,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -457,7 +1486,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.6</v>
       </c>
@@ -465,7 +1494,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.7</v>
       </c>
@@ -473,7 +1502,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.8</v>
       </c>
@@ -481,7 +1510,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.9</v>
       </c>
@@ -489,7 +1518,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -497,7 +1526,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1.5</v>
       </c>
@@ -505,7 +1534,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2</v>
       </c>
@@ -513,7 +1542,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -521,7 +1550,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -529,7 +1558,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3.5</v>
       </c>
@@ -537,7 +1566,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>4</v>
       </c>
@@ -545,7 +1574,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>4.5</v>
       </c>
@@ -556,4 +1585,162 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB42D6B-F6A5-4CAF-81FA-07A0735D7F94}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="3" width="13.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B4">
+        <f>32/1000</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>0.01</v>
+      </c>
+      <c r="B5">
+        <f>51.1/1000</f>
+        <v>5.11E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="B11">
+        <v>0.442</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="B12">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>0.154</v>
+      </c>
+      <c r="B13">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="B14">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="C14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="B15">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>0.23</v>
+      </c>
+      <c r="B16">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="C16">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="B17">
+        <v>0.77</v>
+      </c>
+      <c r="C17">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="B18">
+        <v>1.095</v>
+      </c>
+      <c r="C18">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>0.36</v>
+      </c>
+      <c r="B19">
+        <v>1.111</v>
+      </c>
+      <c r="C19">
+        <v>1191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done current sensing just gotta clean up
</commit_message>
<xml_diff>
--- a/Software/Force Sensor Testing.xlsx
+++ b/Software/Force Sensor Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gripper-Arm\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4951AC26-C337-488C-8B4F-CCA3B663D80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CF1E5-7370-4DBF-984A-B6EC0953A3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1920" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
+    <workbookView xWindow="11168" yWindow="0" windowWidth="11415" windowHeight="14362" activeTab="1" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Load (kg)</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>ADC Reading</t>
-  </si>
-  <si>
-    <t>Voltage (V)</t>
   </si>
 </sst>
 </file>
@@ -110,6 +107,1037 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0914260717410318E-2"/>
+          <c:y val="8.0983887430737825E-2"/>
+          <c:w val="0.87437751531058616"/>
+          <c:h val="0.73577136191309422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12759978744189027"/>
+                  <c:y val="-1.4646749315056553E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$23:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$23:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>242.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>280.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>303.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>343.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>387.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>463.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>512.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>561.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>614.70000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-51CF-4916-8BD6-7E4105B1EB88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="450241984"/>
+        <c:axId val="450236224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="450241984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450236224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="450236224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450241984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>340518</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64293</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>378618</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>92868</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81EA1F41-5FB2-BC3C-311B-A57E09336C6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,17 +1443,17 @@
       <selection activeCell="D22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -433,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0</v>
       </c>
@@ -441,7 +1469,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -449,7 +1477,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -457,7 +1485,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -465,7 +1493,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.4</v>
       </c>
@@ -473,7 +1501,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -481,7 +1509,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.6</v>
       </c>
@@ -489,7 +1517,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.7</v>
       </c>
@@ -497,7 +1525,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.8</v>
       </c>
@@ -505,7 +1533,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.9</v>
       </c>
@@ -513,7 +1541,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -521,7 +1549,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1.5</v>
       </c>
@@ -529,7 +1557,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2</v>
       </c>
@@ -537,7 +1565,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -545,7 +1573,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -553,7 +1581,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3.5</v>
       </c>
@@ -561,7 +1589,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>4</v>
       </c>
@@ -569,7 +1597,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>4.5</v>
       </c>
@@ -584,158 +1612,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB42D6B-F6A5-4CAF-81FA-07A0735D7F94}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="97" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="B4">
-        <f>32/1000</f>
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.01</v>
-      </c>
-      <c r="B5">
-        <f>51.1/1000</f>
-        <v>5.11E-2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="B11">
-        <v>0.442</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="B23">
+        <v>51.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>0.111</v>
+      </c>
+      <c r="B24">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>0.127</v>
+      </c>
+      <c r="B25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="B26">
+        <v>149.19999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27">
         <v>0.14199999999999999</v>
       </c>
-      <c r="B12">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.154</v>
-      </c>
-      <c r="B13">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="C13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="B14">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="C14">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="B15">
-        <v>0.66300000000000003</v>
-      </c>
-      <c r="C15">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0.23</v>
-      </c>
-      <c r="B16">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="C16">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="B17">
-        <v>0.77</v>
-      </c>
-      <c r="C17">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="B18">
-        <v>1.095</v>
-      </c>
-      <c r="C18">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0.36</v>
-      </c>
-      <c r="B19">
-        <v>1.111</v>
-      </c>
-      <c r="C19">
-        <v>1191</v>
+      <c r="B27">
+        <v>179.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>0.158</v>
+      </c>
+      <c r="B28">
+        <v>242.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="B29">
+        <v>280.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>0.17</v>
+      </c>
+      <c r="B30">
+        <v>303.60000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="B31">
+        <v>343.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>0.19</v>
+      </c>
+      <c r="B32">
+        <v>387.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="B33">
+        <v>463.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="B34">
+        <v>512.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="B35">
+        <v>561.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>0.22</v>
+      </c>
+      <c r="B36">
+        <v>614.70000000000005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated force sensor testing data
</commit_message>
<xml_diff>
--- a/Software/Force Sensor Testing.xlsx
+++ b/Software/Force Sensor Testing.xlsx
@@ -1,43 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gripper-Arm\Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiara\Desktop\Projects\Gripper Arm - ROBOTICS CLUB\Gripper-Arm\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CF1E5-7370-4DBF-984A-B6EC0953A3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00508A22-9562-4B42-B981-E3AE4F39ED86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11168" yWindow="0" windowWidth="11415" windowHeight="14362" activeTab="1" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
+    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="10155" activeTab="2" xr2:uid="{59AF105B-DC93-4845-9EB6-60EFE809D8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="FSR_2 Input Test + Sensor 2" sheetId="3" r:id="rId3"/>
+    <sheet name="FSR_1 Input Test + Sensor 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Load (kg)</t>
   </si>
@@ -55,6 +46,33 @@
   </si>
   <si>
     <t>ADC Reading</t>
+  </si>
+  <si>
+    <t>FSR_2 Input Test + Sensor 2</t>
+  </si>
+  <si>
+    <t>ADC_test 1</t>
+  </si>
+  <si>
+    <t>Voltage_test 1 (V)</t>
+  </si>
+  <si>
+    <t>Voltage_test 2 (V)</t>
+  </si>
+  <si>
+    <t>ADC_test 2</t>
+  </si>
+  <si>
+    <t>Voltage_test 3 (V)</t>
+  </si>
+  <si>
+    <t>ADC_test 3</t>
+  </si>
+  <si>
+    <t>Voltage_test 4 (V)</t>
+  </si>
+  <si>
+    <t>ADC_test 4</t>
   </si>
 </sst>
 </file>
@@ -1440,20 +1458,20 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1469,7 +1487,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -1477,7 +1495,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -1485,7 +1503,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -1493,7 +1511,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>0.4</v>
       </c>
@@ -1501,7 +1519,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>0.6</v>
       </c>
@@ -1517,7 +1535,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>0.7</v>
       </c>
@@ -1525,7 +1543,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>0.8</v>
       </c>
@@ -1533,7 +1551,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>0.9</v>
       </c>
@@ -1541,7 +1559,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1549,7 +1567,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>1.5</v>
       </c>
@@ -1557,7 +1575,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1565,7 +1583,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -1573,7 +1591,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1581,7 +1599,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>3.5</v>
       </c>
@@ -1589,7 +1607,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1597,7 +1615,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>4.5</v>
       </c>
@@ -1614,22 +1632,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB42D6B-F6A5-4CAF-81FA-07A0735D7F94}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="97" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="97" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.40625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>9.5000000000000001E-2</v>
       </c>
@@ -1645,7 +1663,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>0.111</v>
       </c>
@@ -1653,7 +1671,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>0.127</v>
       </c>
@@ -1661,7 +1679,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>0.13300000000000001</v>
       </c>
@@ -1669,7 +1687,7 @@
         <v>149.19999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>0.14199999999999999</v>
       </c>
@@ -1677,7 +1695,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>0.158</v>
       </c>
@@ -1685,7 +1703,7 @@
         <v>242.7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>0.16500000000000001</v>
       </c>
@@ -1693,7 +1711,7 @@
         <v>280.2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>0.17</v>
       </c>
@@ -1701,7 +1719,7 @@
         <v>303.60000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>0.18099999999999999</v>
       </c>
@@ -1709,7 +1727,7 @@
         <v>343.7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>0.19</v>
       </c>
@@ -1717,7 +1735,7 @@
         <v>387.3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>0.19800000000000001</v>
       </c>
@@ -1725,7 +1743,7 @@
         <v>463.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>0.20399999999999999</v>
       </c>
@@ -1733,7 +1751,7 @@
         <v>512.9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>0.21099999999999999</v>
       </c>
@@ -1741,7 +1759,7 @@
         <v>561.5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>0.22</v>
       </c>
@@ -1753,4 +1771,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B222E696-F36D-456B-9448-23D85C8B790D}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="15.31640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.31640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.31640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.31640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C3">
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <v>0.12</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>0.13</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>0.129</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4">
+        <v>0.19</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>0.15</v>
+      </c>
+      <c r="E4">
+        <v>46</v>
+      </c>
+      <c r="F4">
+        <v>0.19</v>
+      </c>
+      <c r="G4">
+        <v>109</v>
+      </c>
+      <c r="H4">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="I4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5">
+        <v>0.27</v>
+      </c>
+      <c r="C5">
+        <v>175</v>
+      </c>
+      <c r="D5">
+        <v>0.24</v>
+      </c>
+      <c r="E5">
+        <v>145</v>
+      </c>
+      <c r="F5">
+        <v>0.19</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>0.21</v>
+      </c>
+      <c r="I5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6">
+        <v>0.33</v>
+      </c>
+      <c r="C6">
+        <v>260</v>
+      </c>
+      <c r="D6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E6">
+        <v>210</v>
+      </c>
+      <c r="F6">
+        <v>0.21</v>
+      </c>
+      <c r="G6">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>0.23</v>
+      </c>
+      <c r="I6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>0.39</v>
+      </c>
+      <c r="C7">
+        <v>330</v>
+      </c>
+      <c r="D7">
+        <v>0.26</v>
+      </c>
+      <c r="E7">
+        <v>290</v>
+      </c>
+      <c r="F7">
+        <v>0.25</v>
+      </c>
+      <c r="G7">
+        <v>150</v>
+      </c>
+      <c r="H7">
+        <v>0.26</v>
+      </c>
+      <c r="I7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C8">
+        <v>560</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>450</v>
+      </c>
+      <c r="F8">
+        <v>0.32</v>
+      </c>
+      <c r="G8">
+        <v>320</v>
+      </c>
+      <c r="H8">
+        <v>0.4</v>
+      </c>
+      <c r="I8">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>1.5</v>
+      </c>
+      <c r="B9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C9">
+        <v>549</v>
+      </c>
+      <c r="D9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E9">
+        <v>540</v>
+      </c>
+      <c r="F9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G9">
+        <v>530</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+      <c r="C10">
+        <v>590</v>
+      </c>
+      <c r="D10">
+        <v>0.64</v>
+      </c>
+      <c r="E10">
+        <v>650</v>
+      </c>
+      <c r="F10">
+        <v>0.61</v>
+      </c>
+      <c r="G10">
+        <v>590</v>
+      </c>
+      <c r="H10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I10">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>2.5</v>
+      </c>
+      <c r="B11">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="C11">
+        <v>790</v>
+      </c>
+      <c r="D11">
+        <v>0.68</v>
+      </c>
+      <c r="E11">
+        <v>680</v>
+      </c>
+      <c r="F11">
+        <v>0.71</v>
+      </c>
+      <c r="G11">
+        <v>720</v>
+      </c>
+      <c r="H11">
+        <v>0.63</v>
+      </c>
+      <c r="I11">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>0.82</v>
+      </c>
+      <c r="C12">
+        <v>860</v>
+      </c>
+      <c r="D12">
+        <v>0.71</v>
+      </c>
+      <c r="E12">
+        <v>720</v>
+      </c>
+      <c r="F12">
+        <v>0.76</v>
+      </c>
+      <c r="G12">
+        <v>790</v>
+      </c>
+      <c r="H12">
+        <v>0.71</v>
+      </c>
+      <c r="I12">
+        <v>740</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3453FC4E-5B62-47E0-A5D9-1BF09B4EF45E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>